<commit_message>
I've added functions and updated structure of the project
</commit_message>
<xml_diff>
--- a/data/merged_names.xlsx
+++ b/data/merged_names.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ALRS RX,алроса,alrosa</t>
+          <t>alrs rx,алроса,alrosa</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>AVAN,Авангард,AVANGARD</t>
+          <t>avan,авангард,avangard</t>
         </is>
       </c>
     </row>
@@ -498,7 +498,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PRMB,АКБ Приморье,АКБ "Приморье",банк "Приморье",банк Приморье,primbank,PJSCB "Primorye",PJSCB Primorye,public joint-stock commercial bank "Primorye",bank "Primorye",bank Primorye</t>
+          <t>prmb,акб приморье,акб "приморье",банк "приморье",банк приморье,primbank,pjscb "primorye",pjscb primorye,public joint-stock commercial bank "primorye",bank "primorye",bank primorye</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>VTBR RX,ВТБ,VTB</t>
+          <t>vtbr rx,втб,vtb</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>IRGZ,Иркутскэнерго,ИркЭнерго,Irkutskenergo</t>
+          <t>irgz,иркутскэнерго,иркэнерго,irkutskenergo</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>KZOS,Органический синтез,Казаньоргсинтез,kazanorgsintez</t>
+          <t>kzos,органический синтез,казаньоргсинтез,kazanorgsintez</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>LNZL,Лензолото,Lenzoloto</t>
+          <t>lnzl,лензолото,lenzoloto</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>RUAL RX,Объединённая компания "Русал",русал,rusal</t>
+          <t>rual rx,объединённая компания "русал",русал,rusal</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ENPG RX,ENPL,эн+ груп,En+ Group,EN+ Group Plc</t>
+          <t>enpg rx,enpl,эн+ груп,en+ group,en+ group plc</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>BLNG,Белон ,belon</t>
+          <t>blng,белон ,belon</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>DZRD,Донской завод радиодеталей,ДЗРД</t>
+          <t>dzrd,донской завод радиодеталей,дзрд</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>LVHK,Левенгук,levenhuk</t>
+          <t>lvhk,левенгук,levenhuk</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>LPSB,LPSBG,Липецкая энергосбытовая компания,Липецкая ЭСК,ЛЭСК,lesk</t>
+          <t>lpsb,lpsbg,липецкая энергосбытовая компания,липецкая эск,лэск,lesk</t>
         </is>
       </c>
     </row>
@@ -696,7 +696,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>MRKU                ,Межрегиональная распределительная сетевая компания Урала,МРСК Урала,Россети Урал,rosseti ural</t>
+          <t>mrku                ,межрегиональная распределительная сетевая компания урала,мрск урала,россети урал,rosseti ural</t>
         </is>
       </c>
     </row>
@@ -714,7 +714,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>MSST,Мультисистема,multisistema</t>
+          <t>msst,мультисистема,multisistema</t>
         </is>
       </c>
     </row>
@@ -732,7 +732,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>NPOF,Научно-производственное объединение "Физика",НПО "Физика",НПО Физика,npofizika</t>
+          <t>npof,научно-производственное объединение "физика",нпо "физика",нпо физика,npofizika</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>MGNZ,MGNZG,Соликамский магниевый завод,ОАО "СМЗ",ОАО СМЗ</t>
+          <t>mgnz,mgnzg,соликамский магниевый завод,оао "смз",оао смз</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>AQUA,Инаркт1Р1,Инарктика,Русская Аквакультура,inarctica,Русское море</t>
+          <t>aqua,инаркт1р1,инарктика,русская аквакультура,inarctica,русское море</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ABRD,Абрау – Дюрсо,abraudurso,Абрау Дюрсо</t>
+          <t>abrd,абрау – дюрсо,abraudurso,абрау дюрсо</t>
         </is>
       </c>
     </row>
@@ -804,7 +804,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>UTAR</t>
+          <t>utar</t>
         </is>
       </c>
     </row>
@@ -822,7 +822,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>AKRN RX,акрон,Acron</t>
+          <t>akrn rx,акрон,acron</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>BANE RX</t>
+          <t>bane rx</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>AFKS RX,АФК Система,Система</t>
+          <t>afks rx,афк система,система</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ALNU RX,Алроса,Alrosa</t>
+          <t>alnu rx,алроса,alrosa</t>
         </is>
       </c>
     </row>
@@ -894,7 +894,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>APTK RX</t>
+          <t>aptk rx</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ACKO</t>
+          <t>acko</t>
         </is>
       </c>
     </row>
@@ -930,7 +930,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ASSB,Астраханская ЭСБ</t>
+          <t>assb,астраханская эсб</t>
         </is>
       </c>
     </row>
@@ -948,7 +948,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>AMEZ</t>
+          <t>amez</t>
         </is>
       </c>
     </row>
@@ -966,7 +966,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>AFLT RX,Аэрофлот,Aeroflot</t>
+          <t>aflt rx,аэрофлот,aeroflot</t>
         </is>
       </c>
     </row>
@@ -984,7 +984,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>BSPB RX,Банк Санкт-Петербург,БСПБ,Банк Петербург,СПБ Банк</t>
+          <t>bspb rx,банк санкт-петербург,бспб,банк петербург,спб банк</t>
         </is>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>USBN</t>
+          <t>usbn</t>
         </is>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">BISV                </t>
+          <t xml:space="preserve">bisv                </t>
         </is>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>BELU RX,Белуга,Beluga</t>
+          <t>belu rx,белуга,beluga</t>
         </is>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ALBK</t>
+          <t>albk</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>BRZL</t>
+          <t>brzl</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>VJGZ</t>
+          <t>vjgz</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>VLHZ</t>
+          <t>vlhz</t>
         </is>
       </c>
     </row>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>VGSB</t>
+          <t>vgsb</t>
         </is>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">OGKB                </t>
+          <t xml:space="preserve">ogkb                </t>
         </is>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>VSYD</t>
+          <t>vsyd</t>
         </is>
       </c>
     </row>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>GAZA                ,группа "ГАЗ",группа ГАЗ,ПАО Газ,ПАО "Газ"</t>
+          <t>gaza                ,группа "газ",группа газ,пао газ,пао "газ"</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>GAZC,газкон,газкон-ао</t>
+          <t>gazc,газкон,газкон-ао</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>RTGZ,ПАО "Газпром газораспределение Ростов-на-Дону",rostovoblgaz,Газпром РнД,Ростовоблгаз</t>
+          <t>rtgz,пао "газпром газораспределение ростов-на-дону",rostovoblgaz,газпром рнд,ростовоблгаз</t>
         </is>
       </c>
     </row>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>SIBN RX,ПАО "Газпром нефть",Газпром нефть,Gazprom Neft</t>
+          <t>sibn rx,пао "газпром нефть",газпром нефть,gazprom neft</t>
         </is>
       </c>
     </row>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>GAZP RX,ПАО "Газпром",Газпром,Gazprom,gazp</t>
+          <t>gazp rx,пао "газпром",газпром,gazprom,gazp</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>GAZS,ПАО "ГАЗ-сервис",gas-service</t>
+          <t>gazs,пао "газ-сервис",gas-service</t>
         </is>
       </c>
     </row>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>GTSS,геотек,gseis,ПАО «ГЕОТЕК Сейсморазведка»</t>
+          <t>gtss,геотек,gseis,пао «геотек сейсморазведка»</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>GTRK                ,Глобалтрак,Globaltruck</t>
+          <t>gtrk                ,глобалтрак,globaltruck</t>
         </is>
       </c>
     </row>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>GMKN RX,Норникель,ПАО "Горно-металлургическая компания "Норильский никель",ПАО "ГМК "Норильский никель",Nornickel ,Норильский никель</t>
+          <t>gmkn rx,норникель,пао "горно-металлургическая компания "норильский никель",пао "гмк "норильский никель",nornickel ,норильский никель</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>GRNT,ПАО «Городские Инновационные Технологии,ПАО "ГИТ",Городские Инновационные Технологии,ГИТ</t>
+          <t>grnt,пао «городские инновационные технологии,пао "гит",городские инновационные технологии,гит</t>
         </is>
       </c>
     </row>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>RLMN,Роллман,Rollman</t>
+          <t>rlmn,роллман,rollman</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>SMLT RX,Самолет,Samolet,группа самолет</t>
+          <t>smlt rx,самолет,samolet,группа самолет</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>LSRG RX,ЛСР</t>
+          <t>lsrg rx,лср</t>
         </is>
       </c>
     </row>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>GCHE RX ,Черкизово,Cherkizovo</t>
+          <t>gche rx ,черкизово,cherkizovo</t>
         </is>
       </c>
     </row>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>DASB,ДагСб,Дагестанэнергосбыт,Dagestanskaya Energosbytovaya</t>
+          <t>dasb,дагсб,дагестанэнергосбыт,dagestanskaya energosbytovaya</t>
         </is>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>DVEC,ДЭК,Дальневосточная энергетическая компания</t>
+          <t>dvec,дэк,дальневосточная энергетическая компания</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>FESH                ,ДВМП,FESCO,Дальневосточное морское пароходство</t>
+          <t>fesh                ,двмп,fesco,дальневосточное морское пароходство</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>DSKY RX,Детский мир,Detsky Mir,Детмир</t>
+          <t>dsky rx,детский мир,detsky mir,детмир</t>
         </is>
       </c>
     </row>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>GTLC ,ДжиТиЭл,GTL</t>
+          <t>gtlc ,джитиэл,gtl</t>
         </is>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>EELT                ,Европейская Электротехника,Yevropyeyskaya Elyektrotyekhnika</t>
+          <t>eelt                ,европейская электротехника,yevropyeyskaya elyektrotyekhnika</t>
         </is>
       </c>
     </row>
@@ -1560,7 +1560,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t xml:space="preserve">ZILL                ,Завод имени И.А. Лихачева,ЗИЛ,ZIL,Завод имени Лихачёва </t>
+          <t xml:space="preserve">zill                ,завод имени и.а. лихачева,зил,zil,завод имени лихачёва </t>
         </is>
       </c>
     </row>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>ZVEZ,Звезда,ZVEZDA</t>
+          <t>zvez,звезда,zvezda</t>
         </is>
       </c>
     </row>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>IGST                ,Ижсталь,Ижевский металлургический завод,Izhstal'</t>
+          <t>igst                ,ижсталь,ижевский металлургический завод,izhstal'</t>
         </is>
       </c>
     </row>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>IDVP,инвест-девелопмент,invest-development</t>
+          <t>idvp,инвест-девелопмент,invest-development</t>
         </is>
       </c>
     </row>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>RUSI,Руссинвест,ИК Русс-Инвест ,Russ-Invest,Русс-Инвест,Russinvest ,Русс-Инвест ИК</t>
+          <t>rusi,руссинвест,ик русс-инвест ,russ-invest,русс-инвест,russinvest ,русс-инвест ик</t>
         </is>
       </c>
     </row>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>INGR RX,OPIN,Инград,Ingrad ,Ingr,Инград (ПАО),ПАО Инград</t>
+          <t>ingr rx,opin,инград,ingrad ,ingr,инград (пао),пао инград</t>
         </is>
       </c>
     </row>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>ISKJ                ,ИСКЧ,Институт Стволовых Клеток Человека</t>
+          <t>iskj                ,искч,институт стволовых клеток человека</t>
         </is>
       </c>
     </row>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>IRAO RX,Интер РАО ,Inter Rao,Интер РАО ЕЭС Финанс</t>
+          <t>irao rx,интер рао ,inter rao,интер рао еэс финанс</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>KLSB,КСК,КЛСБ,Калужская сбытовая компания,Калужская СбытКомп,Kalujskaya Sbytovaya</t>
+          <t>klsb,кск,клсб,калужская сбытовая компания,калужская сбыткомп,kalujskaya sbytovaya</t>
         </is>
       </c>
     </row>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve">KMAZ RX,Камаз,Kamaz </t>
+          <t xml:space="preserve">kmaz rx,камаз,kamaz </t>
         </is>
       </c>
     </row>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>KUNF,Кузоцм,Kuzocm</t>
+          <t>kunf,кузоцм,kuzocm</t>
         </is>
       </c>
     </row>
@@ -1758,7 +1758,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>TGKD,АО Квадра,quadra,квадра,пао квадра</t>
+          <t>tgkd,ао квадра,quadra,квадра,пао квадра</t>
         </is>
       </c>
     </row>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>KMEZ,ПАО КМЗ,Ковровский мехзд,Ковровский механический завод,kvmz</t>
+          <t>kmez,пао кмз,ковровский мехзд,ковровский механический завод,kvmz</t>
         </is>
       </c>
     </row>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>KSGR                ,ПАО кокс,кокс,koks</t>
+          <t>ksgr                ,пао кокс,кокс,koks</t>
         </is>
       </c>
     </row>
@@ -1812,7 +1812,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>VSMO                ,Корпорация ВСМПО-АВИСМА,ВСМПО-АВИСМА,VSMPO-AVISMA Corporation,VSMPO-AVISMA,ВСМПО-АВСМ,ВСМПО</t>
+          <t>vsmo                ,корпорация всмпо-ависма,всмпо-ависма,vsmpo-avisma corporation,vsmpo-avisma,всмпо-авсм,всмпо</t>
         </is>
       </c>
     </row>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>KOGK                ,Коршуновский гок,Korshunov Mining Plant,Korgok</t>
+          <t>kogk                ,коршуновский гок,korshunov mining plant,korgok</t>
         </is>
       </c>
     </row>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>KMTZ                ,Косогорский металлургический завод,ПАО КМЗ,KGIW</t>
+          <t>kmtz                ,косогорский металлургический завод,пао кмз,kgiw</t>
         </is>
       </c>
     </row>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>KTSB,КСК,Костромская сбытовая компания,Kostromskaya sbytovaya kompaniya,KSK</t>
+          <t>ktsb,кск,костромская сбытовая компания,kostromskaya sbytovaya kompaniya,ksk</t>
         </is>
       </c>
     </row>
@@ -1884,7 +1884,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>KZMS,КЗМС,Краснокамский завод металлических сеток,Россет,Rosset</t>
+          <t>kzms,кзмс,краснокамский завод металлических сеток,россет,rosset</t>
         </is>
       </c>
     </row>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>KRSB,Красноярскэнергосбыт,krsk-sbit</t>
+          <t>krsb,красноярскэнергосбыт,krsk-sbit</t>
         </is>
       </c>
     </row>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>KBTK,Кузбасская топливная компания,КТК,KTK,ПАО КТК</t>
+          <t>kbtk,кузбасская топливная компания,ктк,ktk,пао ктк</t>
         </is>
       </c>
     </row>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>KAZT,КуйбышевАзот,kuazot,Куйбазот</t>
+          <t>kazt,куйбышевазот,kuazot,куйбазот</t>
         </is>
       </c>
     </row>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>KGKC,Курганская генерирующая компания,Курганская ГК,КГК,ПАО КГК,KGK,Kurgancskaya Generiruyushaya</t>
+          <t>kgkc,курганская генерирующая компания,курганская гк,кгк,пао кгк,kgk,kurgancskaya generiruyushaya</t>
         </is>
       </c>
     </row>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>MVID RX,Мвидео,Mvideo</t>
+          <t>mvid rx,мвидео,mvideo</t>
         </is>
       </c>
     </row>
@@ -1992,7 +1992,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>MGNT RX,Магнит ,Magnit ,Mgnt ,ПАО Магнит,Магнит ПАО</t>
+          <t>mgnt rx,магнит ,magnit ,mgnt ,пао магнит,магнит пао</t>
         </is>
       </c>
     </row>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>MAGN RX,ММК,Magnitigorskiy Metallurgicheskiy,Магнитогорский металлургический комбинат,Магнитка</t>
+          <t>magn rx,ммк,magnitigorskiy metallurgicheskiy,магнитогорский металлургический комбинат,магнитка</t>
         </is>
       </c>
     </row>
@@ -2028,7 +2028,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>MFON RX,Мегафон,Megafon,ПАО Мегафон,Мегафон ПАО</t>
+          <t>mfon rx,мегафон,megafon,пао мегафон,мегафон пао</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>ODVA</t>
+          <t>odva</t>
         </is>
       </c>
     </row>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>GEMA</t>
+          <t>gema</t>
         </is>
       </c>
     </row>
@@ -2082,7 +2082,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>MRKZ</t>
+          <t>mrkz</t>
         </is>
       </c>
     </row>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>MRKP</t>
+          <t>mrkp</t>
         </is>
       </c>
     </row>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>MRKC</t>
+          <t>mrkc</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>MERF</t>
+          <t>merf</t>
         </is>
       </c>
     </row>
@@ -2154,7 +2154,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>MTKB</t>
+          <t>mtkb</t>
         </is>
       </c>
     </row>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>MTLR RX,мечел,mechel,mtlrp</t>
+          <t>mtlr rx,мечел,mechel,mtlrp</t>
         </is>
       </c>
     </row>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>MTSS RX,MTC,МТС</t>
+          <t>mtss rx,mtc,мтс</t>
         </is>
       </c>
     </row>
@@ -2208,7 +2208,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>MRSB</t>
+          <t>mrsb</t>
         </is>
       </c>
     </row>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>MORI</t>
+          <t>mori</t>
         </is>
       </c>
     </row>
@@ -2244,7 +2244,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>MOEX RX,Мосбиржа,Московская биржа</t>
+          <t>moex rx,мосбиржа,московская биржа</t>
         </is>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t xml:space="preserve">MGTS RX </t>
+          <t xml:space="preserve">mgts rx </t>
         </is>
       </c>
     </row>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>KROT,KROTP</t>
+          <t>krot,krotp</t>
         </is>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>NSVZ,наука-связь</t>
+          <t>nsvz,наука-связь</t>
         </is>
       </c>
     </row>
@@ -2334,7 +2334,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>IRKT RX</t>
+          <t>irkt rx</t>
         </is>
       </c>
     </row>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>UWGN RX,Объединенная Вагонная Компания</t>
+          <t>uwgn rx,объединенная вагонная компания</t>
         </is>
       </c>
     </row>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>NFAZ,нефаз,Нефтекамский автозавод</t>
+          <t>nfaz,нефаз,нефтекамский автозавод</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>LKOH RX,ЛУКОЙЛ</t>
+          <t>lkoh rx,лукойл</t>
         </is>
       </c>
     </row>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>ROSN RX,роснефть,rosneft</t>
+          <t>rosn rx,роснефть,rosneft</t>
         </is>
       </c>
     </row>
@@ -2424,7 +2424,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>NKNCP,NKNC,Нижнекамскнефтехим</t>
+          <t>nkncp,nknc,нижнекамскнефтехим</t>
         </is>
       </c>
     </row>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>NKSHP,NKSH,Нижнекамскшина</t>
+          <t>nkshp,nksh,нижнекамскшина</t>
         </is>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>NVTK RX,Новатэк,Novatek</t>
+          <t>nvtk rx,новатэк,novatek</t>
         </is>
       </c>
     </row>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>NLMK RX,НЛМК</t>
+          <t>nlmk rx,нлмк</t>
         </is>
       </c>
     </row>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>NKHP,новороссийский комбинат хлебопродуктов,нкхп</t>
+          <t>nkhp,новороссийский комбинат хлебопродуктов,нкхп</t>
         </is>
       </c>
     </row>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>UNAC RX,ПАО ОАК,ПАО "ОАК",объединенная авиастроительная корпорация</t>
+          <t>unac rx,пао оак,пао "оак",объединенная авиастроительная корпорация</t>
         </is>
       </c>
     </row>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>UCSS,Кредитные системы,Объединенные Кредитные Системы</t>
+          <t>ucss,кредитные системы,объединенные кредитные системы</t>
         </is>
       </c>
     </row>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>SATR,Сатурн,ОДК Сатурн,ОДК-Сатурн,ОДК_Сатурн</t>
+          <t>satr,сатурн,одк сатурн,одк-сатурн,одк_сатурн</t>
         </is>
       </c>
     </row>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>ORUP,ОР ГРУПП,ПАО ОР</t>
+          <t>orup,ор групп,пао ор</t>
         </is>
       </c>
     </row>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>paza,Павловский автобус,Павл Автобус,ПавлБус</t>
+          <t>paza,павловский автобус,павл автобус,павлбус</t>
         </is>
       </c>
     </row>
@@ -2640,7 +2640,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>PMSBP,PMSB,ПЕРМЭНЕРГОСБЫТ,Пермская энергосбытовая компания</t>
+          <t>pmsbp,pmsb,пермэнергосбыт,пермская энергосбытовая компания</t>
         </is>
       </c>
     </row>
@@ -2658,7 +2658,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>PIKK RX,ПИК СЗ</t>
+          <t>pikk rx,пик сз</t>
         </is>
       </c>
     </row>
@@ -2676,7 +2676,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>PLZL RX,Полюс</t>
+          <t>plzl rx,полюс</t>
         </is>
       </c>
     </row>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>RKKE                ,Энергия,РКК Энергия,РКК «Энергия»</t>
+          <t>rkke                ,энергия,ркк энергия,ркк «энергия»</t>
         </is>
       </c>
     </row>
@@ -2712,7 +2712,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>RASP RX ,ПАО «Распадская»,Распадская</t>
+          <t>rasp rx ,пао «распадская»,распадская</t>
         </is>
       </c>
     </row>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>RBCM,РосБизнесКонсалтинг,ГК «РосБизнесКонсалтинг»,Рос Бизнес Консалтинг</t>
+          <t>rbcm,росбизнесконсалтинг,гк «росбизнесконсалтинг»,рос бизнес консалтинг</t>
         </is>
       </c>
     </row>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>CHGZ,РН-Западная Сибирь</t>
+          <t>chgz,рн-западная сибирь</t>
         </is>
       </c>
     </row>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>RGSC,Росгосстрах Банк,Банк Росгосстрах,РГС Банк,Росгосстрах</t>
+          <t>rgsc,росгосстрах банк,банк росгосстрах,ргс банк,росгосстрах</t>
         </is>
       </c>
     </row>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>ROST,РОСИНТЕР РЕСТОРАНТС ХОЛДИНГ,РОСИНТЕР,Rosinter</t>
+          <t>rost,росинтер ресторантс холдинг,росинтер,rosinter</t>
         </is>
       </c>
     </row>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>mrkv,Россети Волга</t>
+          <t>mrkv,россети волга</t>
         </is>
       </c>
     </row>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>kube,Россети Кубань</t>
+          <t>kube,россети кубань</t>
         </is>
       </c>
     </row>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>lsng,Россети Ленэнерго</t>
+          <t>lsng,россети ленэнерго</t>
         </is>
       </c>
     </row>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>MSRS                ,Россети Московский регион</t>
+          <t>msrs                ,россети московский регион</t>
         </is>
       </c>
     </row>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>MRKK                ,Россети Северный Кавказ</t>
+          <t>mrkk                ,россети северный кавказ</t>
         </is>
       </c>
     </row>
@@ -2892,7 +2892,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>MRKS,Россети Сибирь</t>
+          <t>mrks,россети сибирь</t>
         </is>
       </c>
     </row>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>MRKY</t>
+          <t>mrky</t>
         </is>
       </c>
     </row>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>RSTI RX,Российские сети</t>
+          <t>rsti rx,российские сети</t>
         </is>
       </c>
     </row>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>RTKM RX,ростелеком</t>
+          <t>rtkm rx,ростелеком</t>
         </is>
       </c>
     </row>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t xml:space="preserve">RUGR                </t>
+          <t xml:space="preserve">rugr                </t>
         </is>
       </c>
     </row>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t xml:space="preserve">ROLO                </t>
+          <t xml:space="preserve">rolo                </t>
         </is>
       </c>
     </row>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t xml:space="preserve">RUSP                </t>
+          <t xml:space="preserve">rusp                </t>
         </is>
       </c>
     </row>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>RZSB</t>
+          <t>rzsb</t>
         </is>
       </c>
     </row>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>KRKN,KRKNP</t>
+          <t>krkn,krknp</t>
         </is>
       </c>
     </row>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>SAREP,SARE,Саратовэнерго</t>
+          <t>sarep,sare,саратовэнерго</t>
         </is>
       </c>
     </row>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>SFIN RX</t>
+          <t>sfin rx</t>
         </is>
       </c>
     </row>
@@ -3090,7 +3090,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>SBER RX,Sberbank,Sber,сбербанк ,сбер</t>
+          <t>sber rx,sberbank,sber,сбербанк ,сбер</t>
         </is>
       </c>
     </row>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>SVET,Светофор Групп,Группа светофор</t>
+          <t>svet,светофор групп,группа светофор</t>
         </is>
       </c>
     </row>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>CHMF RX,северсталь</t>
+          <t>chmf rx,северсталь</t>
         </is>
       </c>
     </row>
@@ -3144,7 +3144,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>SELG                ,селигдар</t>
+          <t>selg                ,селигдар</t>
         </is>
       </c>
     </row>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>SIBG</t>
+          <t>sibg</t>
         </is>
       </c>
     </row>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>MFGS</t>
+          <t>mfgs</t>
         </is>
       </c>
     </row>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>JNOS,JNOSP</t>
+          <t>jnos,jnosp</t>
         </is>
       </c>
     </row>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>FLOT RX,совкомфлот</t>
+          <t>flot rx,совкомфлот</t>
         </is>
       </c>
     </row>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>SVAV RX,соллерс,sollers,северсталь-авто</t>
+          <t>svav rx,соллерс,sollers,северсталь-авто</t>
         </is>
       </c>
     </row>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>STSB</t>
+          <t>stsb</t>
         </is>
       </c>
     </row>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>SNGS RX,сургутнефтегаз</t>
+          <t>sngs rx,сургутнефтегаз</t>
         </is>
       </c>
     </row>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>KRKOP,ткз Красный котельщик,ткз "Красный котельщик",Красный котельщик ,PJSC Krasny Kotelshchik,Krasny Kotelshchik</t>
+          <t>krkop,ткз красный котельщик,ткз "красный котельщик",красный котельщик ,pjsc krasny kotelshchik,krasny kotelshchik</t>
         </is>
       </c>
     </row>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>TASBP,Тамбовэнергосбыт,Тамбовская энергосбытовая компания,TASB</t>
+          <t>tasbp,тамбовэнергосбыт,тамбовская энергосбытовая компания,tasb</t>
         </is>
       </c>
     </row>
@@ -3324,7 +3324,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>TATN RX,Татнефть,Tatneft</t>
+          <t>tatn rx,татнефть,tatneft</t>
         </is>
       </c>
     </row>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>TTLK                ,Таттелеком,tattelecom</t>
+          <t>ttlk                ,таттелеком,tattelecom</t>
         </is>
       </c>
     </row>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>TGKN                ,ТГК-14,TGC-14,TGK-14</t>
+          <t>tgkn                ,тгк-14,tgc-14,tgk-14</t>
         </is>
       </c>
     </row>
@@ -3378,7 +3378,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>TGKA                ,ТГК-1,TGC-1,TGK-1</t>
+          <t>tgka                ,тгк-1,tgc-1,tgk-1</t>
         </is>
       </c>
     </row>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>TGKB,ТГК-2,TGC-2,TGK-2</t>
+          <t>tgkb,тгк-2,tgc-2,tgk-2</t>
         </is>
       </c>
     </row>
@@ -3414,7 +3414,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>VRSB,ТНС энерго Воронеж,VRSBP</t>
+          <t>vrsb,тнс энерго воронеж,vrsbp</t>
         </is>
       </c>
     </row>
@@ -3432,7 +3432,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>KBSB,ТНС энерго Кубань,KBSBP,KBSBP</t>
+          <t>kbsb,тнс энерго кубань,kbsbp,kbsbp</t>
         </is>
       </c>
     </row>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>MISB,ТНС энерго Марий Эл,MISBP</t>
+          <t>misb,тнс энерго марий эл,misbp</t>
         </is>
       </c>
     </row>
@@ -3468,7 +3468,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>NNSB,ТНС энерго Нижний Новгород,NNSB,ТНС энерго Нижний Новг,NNSBP</t>
+          <t>nnsb,тнс энерго нижний новгород,nnsb,тнс энерго нижний новг,nnsbp</t>
         </is>
       </c>
     </row>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>RTSB,ТНС энерго Ростов-на-Дону,RTSB,ТНС энерго Ростов,RTSBP</t>
+          <t>rtsb,тнс энерго ростов-на-дону,rtsb,тнс энерго ростов,rtsbp</t>
         </is>
       </c>
     </row>
@@ -3504,7 +3504,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>YRSB,ТНС энерго Ярославль,YRSB,YRSBP</t>
+          <t>yrsb,тнс энерго ярославль,yrsb,yrsbp</t>
         </is>
       </c>
     </row>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>TORS,Томская распределительная компания,Россети Томск,ТРК,TORS</t>
+          <t>tors,томская распределительная компания,россети томск,трк,tors</t>
         </is>
       </c>
     </row>
@@ -3540,7 +3540,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>TRNFP RX,Транснефть,transneft</t>
+          <t>trnfp rx,транснефть,transneft</t>
         </is>
       </c>
     </row>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>TRFM,ТрансФин,transfin</t>
+          <t>trfm,трансфин,transfin</t>
         </is>
       </c>
     </row>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>TRMK RX,ТМК,OAO TMK,TMK,Трубная Металлургическая Компания</t>
+          <t>trmk rx,тмк,oao tmk,tmk,трубная металлургическая компания</t>
         </is>
       </c>
     </row>
@@ -3594,7 +3594,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>TUZA,ПАО «ТЗА»,ПАО ТЗА,тза,Туймазинский завод автобетоновозов,не TZA -- есть американский тикер</t>
+          <t>tuza,пао «тза»,пао тза,тза,туймазинский завод автобетоновозов,не tza -- есть американский тикер</t>
         </is>
       </c>
     </row>
@@ -3612,7 +3612,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>TUCH,Тучковский КСМ,ТКСМ</t>
+          <t>tuch,тучковский ксм,тксм</t>
         </is>
       </c>
     </row>
@@ -3630,7 +3630,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>UKUZ,ПАО «Южный Кузбасс»,ПАО Южный Кузбасс,Southern Kuzbass Coal Company,Южный Кузбасс</t>
+          <t>ukuz,пао «южный кузбасс»,пао южный кузбасс,southern kuzbass coal company,южный кузбасс</t>
         </is>
       </c>
     </row>
@@ -3648,7 +3648,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>ARSA,ARSA,Арсагера,arsagera(не встречал упоминаний)</t>
+          <t>arsa,arsa,арсагера,arsagera(не встречал упоминаний)</t>
         </is>
       </c>
     </row>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>URKA RX,uralkali,Уралкалий,URKA</t>
+          <t>urka rx,uralkali,уралкалий,urka</t>
         </is>
       </c>
     </row>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>URKZ                ,Уральская кузница,Urals Stampings Plant</t>
+          <t>urkz                ,уральская кузница,urals stampings plant</t>
         </is>
       </c>
     </row>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>LIFE                ,Фармсинтез,Pharmsynthez,Фарм-синтез,ПАО Фармсинтез</t>
+          <t>life                ,фармсинтез,pharmsynthez,фарм-синтез,пао фармсинтез</t>
         </is>
       </c>
     </row>
@@ -3720,7 +3720,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>HYDR RX,Русгидро,RusHydro,ПАО РусГидро</t>
+          <t>hydr rx,русгидро,rushydro,пао русгидро</t>
         </is>
       </c>
     </row>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>FEES RX,Россети ФСК ЕЭС,AO FGC UES,ПАО Россети,ПАО ФСК ЕЭС,ФСК ЕЭС</t>
+          <t>fees rx,россети фск еэс,ao fgc ues,пао россети,пао фск еэс,фск еэс</t>
         </is>
       </c>
     </row>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>PHOR RX,Фосагро,Phosagro</t>
+          <t>phor rx,фосагро,phosagro</t>
         </is>
       </c>
     </row>
@@ -3774,7 +3774,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>HIMCP RX,Химпром,himprom,ПАО Химпром</t>
+          <t>himcp rx,химпром,himprom,пао химпром</t>
         </is>
       </c>
     </row>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>WTCM RX,ЦМТ,WTC,Центр международной торговли,World trade center</t>
+          <t>wtcm rx,цмт,wtc,центр международной торговли,world trade center</t>
         </is>
       </c>
     </row>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>TRCN RX,Трансконтейнер,Transcontainer,ПАО Трансконейнер</t>
+          <t>trcn rx,трансконтейнер,transcontainer,пао трансконейнер</t>
         </is>
       </c>
     </row>
@@ -3828,7 +3828,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>CNTL RX,Центральный телеграф,Central Telegraph,ПАО Центральный телеграф</t>
+          <t>cntl rx,центральный телеграф,central telegraph,пао центральный телеграф</t>
         </is>
       </c>
     </row>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>PRFN RX            ,ЧЗПСН-Профнастил,ПАО ЧЗПСН-Профнастил,Челябинский завод профилированного стального настила</t>
+          <t>prfn rx            ,чзпсн-профнастил,пао чзпсн-профнастил,челябинский завод профилированного стального настила</t>
         </is>
       </c>
     </row>
@@ -3864,7 +3864,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>CKPZ RX,ЧКПЗ,OAO Chelyabinsk Forge-and-Press Plant,ПАО Челябинский кузнечно-прессовый завод</t>
+          <t>ckpz rx,чкпз,oao chelyabinsk forge-and-press plant,пао челябинский кузнечно-прессовый завод</t>
         </is>
       </c>
     </row>
@@ -3882,7 +3882,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>CHMK RX,ЧМК,Chelyabinsk Metallurgical Plant,ПАО ЧМК,Челябинский металлургический комбинат,ChMK</t>
+          <t>chmk rx,чмк,chelyabinsk metallurgical plant,пао чмк,челябинский металлургический комбинат,chmk</t>
         </is>
       </c>
     </row>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>CHEP RX,ЧТПЗ,Chelyabinsk Pipe Rolling Plant,ПАО ЧТПЗ,Челябинский трубопрокатный завод</t>
+          <t>chep rx,чтпз,chelyabinsk pipe rolling plant,пао чтпз,челябинский трубопрокатный завод</t>
         </is>
       </c>
     </row>
@@ -3918,7 +3918,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>ELTZ RX                ,Электроцинк,Electrozink,ПАО Электроцинк</t>
+          <t>eltz rx                ,электроцинк,electrozink,пао электроцинк</t>
         </is>
       </c>
     </row>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>ENRU RX,Энел Россия,Enel Russia,ПАО Энел Россия,elfv</t>
+          <t>enru rx,энел россия,enel russia,пао энел россия,elfv</t>
         </is>
       </c>
     </row>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>UNKL RX            ,Южуралникель,Unickel,Комбинат Южуралникель,ПАО Комбинат Южуралникель</t>
+          <t>unkl rx            ,южуралникель,unickel,комбинат южуралникель,пао комбинат южуралникель</t>
         </is>
       </c>
     </row>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>UPRO RX,Юнипро,unipro,ПАО Юнипро</t>
+          <t>upro rx,юнипро,unipro,пао юнипро</t>
         </is>
       </c>
     </row>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>YAKG RX,ЯТЭК,Yatec,Якутская топливно-энергетическая компания,ПАО Якутская топливно-энергетическая компания</t>
+          <t>yakg rx,ятэк,yatec,якутская топливно-энергетическая компания,пао якутская топливно-энергетическая компания</t>
         </is>
       </c>
     </row>
@@ -4008,7 +4008,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>YKEN RX,Якутскэнерго,Yakutskenergo,ПАО Якутскэнерго</t>
+          <t>yken rx,якутскэнерго,yakutskenergo,пао якутскэнерго</t>
         </is>
       </c>
     </row>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>VZRZ RX,Банк Возрождение ,Vozrozhdenie Bank,ПАО Банк Возрождение</t>
+          <t>vzrz rx,банк возрождение ,vozrozhdenie bank,пао банк возрождение</t>
         </is>
       </c>
     </row>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>KUZB RX,Банк Кузнецкий,kuzbank,ПАО Банк Кузнецкий</t>
+          <t>kuzb rx,банк кузнецкий,kuzbank,пао банк кузнецкий</t>
         </is>
       </c>
     </row>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>SGZH RX,сегежа,segezha,Сегежа групп,Segezha Group</t>
+          <t>sgzh rx,сегежа,segezha,сегежа групп,segezha group</t>
         </is>
       </c>
     </row>
@@ -4080,7 +4080,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>TNSE RX,ТНС энерго,TNS energo,ПАО ГК ТНС энерго</t>
+          <t>tnse rx,тнс энерго,tns energo,пао гк тнс энерго</t>
         </is>
       </c>
     </row>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>DIOD RX,Диод,DIOD Plant of Ecological Technics and Ecomeals,ПАО Диод ,Завод экологической техники и экопитания Диод</t>
+          <t>diod rx,диод,diod plant of ecological technics and ecomeals,пао диод ,завод экологической техники и экопитания диод</t>
         </is>
       </c>
     </row>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>MOBB</t>
+          <t>mobb</t>
         </is>
       </c>
     </row>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>NAUK</t>
+          <t>nauk</t>
         </is>
       </c>
     </row>
@@ -4152,7 +4152,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t xml:space="preserve">RNFT                </t>
+          <t xml:space="preserve">rnft                </t>
         </is>
       </c>
     </row>
@@ -4170,7 +4170,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>OMZZP,OMZZ</t>
+          <t>omzzp,omzz</t>
         </is>
       </c>
     </row>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>ROSB</t>
+          <t>rosb</t>
         </is>
       </c>
     </row>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>RGSS</t>
+          <t>rgss</t>
         </is>
       </c>
     </row>
@@ -4224,7 +4224,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>KCHEP,KCHE</t>
+          <t>kchep,kche</t>
         </is>
       </c>
     </row>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>MAGEP,MAGE</t>
+          <t>magep,mage</t>
         </is>
       </c>
     </row>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>MSNG                ,мосэнерго,московская энергетическая компания</t>
+          <t>msng                ,мосэнерго,московская энергетическая компания</t>
         </is>
       </c>
     </row>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>SAGO,самарэнерго</t>
+          <t>sago,самарэнерго</t>
         </is>
       </c>
     </row>
@@ -4296,7 +4296,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>SLEN,сахалинэнерго</t>
+          <t>slen,сахалинэнерго</t>
         </is>
       </c>
     </row>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>ETLN LI,Эталон Груп,Группа Эталон</t>
+          <t>etln li,эталон груп,группа эталон</t>
         </is>
       </c>
     </row>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>FIXP RX,Fix Price,FixPrice</t>
+          <t>fixp rx,fix price,fixprice</t>
         </is>
       </c>
     </row>
@@ -4350,7 +4350,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>GLTR LI,Globaltrans,Глобалтранс</t>
+          <t>gltr li,globaltrans,глобалтранс</t>
         </is>
       </c>
     </row>
@@ -4368,7 +4368,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>HHRU RX,Headhunter</t>
+          <t>hhru rx,headhunter</t>
         </is>
       </c>
     </row>
@@ -4386,7 +4386,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>HMSG</t>
+          <t>hmsg</t>
         </is>
       </c>
     </row>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>MAIL LI,VKCO,Вконтакте,ВК,VK Group</t>
+          <t>mail li,vkco,вконтакте,вк,vk group</t>
         </is>
       </c>
     </row>
@@ -4422,7 +4422,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>MDMG RX,MD Medical</t>
+          <t>mdmg rx,md medical</t>
         </is>
       </c>
     </row>
@@ -4440,7 +4440,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>TCS LI,TCSG,TCS Group,Tinkoff,Тинькофф</t>
+          <t>tcs li,tcsg,tcs group,tinkoff,тинькофф</t>
         </is>
       </c>
     </row>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>OKEY RX</t>
+          <t>okey rx</t>
         </is>
       </c>
     </row>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>FIVE LI,Х5 групп,X5 Group</t>
+          <t>five li,х5 групп,x5 group</t>
         </is>
       </c>
     </row>
@@ -4494,7 +4494,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>QIWI RX,АО Киви</t>
+          <t>qiwi rx,ао киви</t>
         </is>
       </c>
     </row>
@@ -4512,7 +4512,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>LNTA,LENT</t>
+          <t>lnta,lent</t>
         </is>
       </c>
     </row>
@@ -4530,7 +4530,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>OZON RX</t>
+          <t>ozon rx</t>
         </is>
       </c>
     </row>
@@ -4548,7 +4548,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>AGRO RX,Русагро,Rusagro</t>
+          <t>agro rx,русагро,rusagro</t>
         </is>
       </c>
     </row>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>RTSD</t>
+          <t>rtsd</t>
         </is>
       </c>
     </row>
@@ -4584,7 +4584,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>NORD,Nordgold</t>
+          <t>nord,nordgold</t>
         </is>
       </c>
     </row>
@@ -4602,7 +4602,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>POGR,Petropavl,"Петропавловск"</t>
+          <t>pogr,petropavl,"петропавловск"</t>
         </is>
       </c>
     </row>
@@ -4620,7 +4620,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>POLY RX,polymetal,полиметалл</t>
+          <t>poly rx,polymetal,полиметалл</t>
         </is>
       </c>
     </row>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>YNDX RX,Яндекс,Yandex</t>
+          <t>yndx rx,яндекс,yandex</t>
         </is>
       </c>
     </row>
@@ -4656,7 +4656,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>SFTL                ,softline,софтлайн,Noventiq</t>
+          <t>sftl                ,softline,софтлайн,noventiq</t>
         </is>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>VEON                ,ВЕОН</t>
+          <t>veon                ,веон</t>
         </is>
       </c>
     </row>
@@ -4692,7 +4692,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>POSI                ,Positive tech,группа позитив,гр. Позитив,Positive Group</t>
+          <t>posi                ,positive tech,группа позитив,гр. позитив,positive group</t>
         </is>
       </c>
     </row>
@@ -4710,7 +4710,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>CIAN                ,cian,циан</t>
+          <t>cian                ,cian,циан</t>
         </is>
       </c>
     </row>
@@ -4728,7 +4728,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>WUSH                ,Whoosh,Вуш</t>
+          <t>wush                ,whoosh,вуш</t>
         </is>
       </c>
     </row>
@@ -4746,7 +4746,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>SPBE,СПБ Биржа</t>
+          <t>spbe,спб биржа</t>
         </is>
       </c>
     </row>
@@ -4764,7 +4764,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>GLPR                ,Globalports,Глобалпортс</t>
+          <t>glpr                ,globalports,глобалпортс</t>
         </is>
       </c>
     </row>
@@ -4782,7 +4782,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>RENI,Ренессанс Страхование</t>
+          <t>reni,ренессанс страхование</t>
         </is>
       </c>
     </row>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>ASTR,Гк Астра,Группа Астра,Astra,Астра</t>
+          <t>astr,гк астра,группа астра,astra,астра</t>
         </is>
       </c>
     </row>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>AQUA,Инарктика,Русское море,Русская аквакультура,Аквакультура</t>
+          <t>aqua,инарктика,русское море,русская аквакультура,аквакультура</t>
         </is>
       </c>
     </row>
@@ -4836,7 +4836,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>UGLD,ЮГК</t>
+          <t>ugld,югк</t>
         </is>
       </c>
     </row>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>ABIO,Артген Биотех,Артген,iАРТГЕН</t>
+          <t>abio,артген биотех,артген,iартген</t>
         </is>
       </c>
     </row>
@@ -4872,7 +4872,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>GECO,Genetico,iГенетико</t>
+          <t>geco,genetico,iгенетико</t>
         </is>
       </c>
     </row>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>CARM,Смарттехгрупп,ПАО "СТГ"</t>
+          <t>carm,смарттехгрупп,пао "стг"</t>
         </is>
       </c>
     </row>
@@ -4908,7 +4908,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>HNFG,Хендерсон</t>
+          <t>hnfg,хендерсон</t>
         </is>
       </c>
     </row>
@@ -4926,7 +4926,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>SVCB,Sovcombank</t>
+          <t>svcb,sovcombank</t>
         </is>
       </c>
     </row>
@@ -4944,7 +4944,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>EUTR,АЗС Трасса,АЗС "Трасса",АЗС «Трасса»</t>
+          <t>eutr,азс трасса,азс "трасса",азс «трасса»</t>
         </is>
       </c>
     </row>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>DELI,Делимобил,Каршеринг Рус,delimobil,ПАО "Каршеринг Руссия","Каршеринг Руссия", ПАО</t>
+          <t>deli,делимобил,каршеринг рус,delimobil,пао "каршеринг руссия","каршеринг руссия", пао</t>
         </is>
       </c>
     </row>
@@ -4980,7 +4980,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>DIAS,Diasoft</t>
+          <t>dias,diasoft</t>
         </is>
       </c>
     </row>

</xml_diff>